<commit_message>
Zaimplementowano barebone poprawnego zapisywania danych z openpyxl
</commit_message>
<xml_diff>
--- a/pyxltext.xlsx
+++ b/pyxltext.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU1"/>
+  <dimension ref="A1:AU9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,6 +658,582 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>253</v>
+      </c>
+      <c r="J2" t="n">
+        <v>253</v>
+      </c>
+      <c r="K2" t="n">
+        <v>246</v>
+      </c>
+      <c r="L2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N2" t="n">
+        <v>246</v>
+      </c>
+      <c r="O2" t="n">
+        <v>246</v>
+      </c>
+      <c r="P2" t="n">
+        <v>253</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>246</v>
+      </c>
+      <c r="R2" t="n">
+        <v>246</v>
+      </c>
+      <c r="S2" t="n">
+        <v>253</v>
+      </c>
+      <c r="T2" t="n">
+        <v>253</v>
+      </c>
+      <c r="U2" t="n">
+        <v>253</v>
+      </c>
+      <c r="V2" t="n">
+        <v>246</v>
+      </c>
+      <c r="W2" t="n">
+        <v>246</v>
+      </c>
+      <c r="X2" t="n">
+        <v>246</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>254</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>254</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>254</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>49699</v>
+      </c>
+      <c r="B8" t="n">
+        <v>49192</v>
+      </c>
+      <c r="C8" t="n">
+        <v>49192</v>
+      </c>
+      <c r="D8" t="n">
+        <v>49192</v>
+      </c>
+      <c r="E8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="F8" t="n">
+        <v>36897</v>
+      </c>
+      <c r="G8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="H8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="L8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="M8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="N8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="O8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="R8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="W8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="X8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>32768</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>257</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>32801</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>129</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>257</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>49161</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>257</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>32800</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>20617</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>4225</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>32769</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>32801</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>63</v>
+      </c>
+      <c r="B9" t="n">
+        <v>63</v>
+      </c>
+      <c r="C9" t="n">
+        <v>63</v>
+      </c>
+      <c r="D9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E9" t="n">
+        <v>63</v>
+      </c>
+      <c r="F9" t="n">
+        <v>63</v>
+      </c>
+      <c r="G9" t="n">
+        <v>63</v>
+      </c>
+      <c r="H9" t="n">
+        <v>63</v>
+      </c>
+      <c r="I9" t="n">
+        <v>45</v>
+      </c>
+      <c r="J9" t="n">
+        <v>45</v>
+      </c>
+      <c r="K9" t="n">
+        <v>63</v>
+      </c>
+      <c r="L9" t="n">
+        <v>63</v>
+      </c>
+      <c r="M9" t="n">
+        <v>63</v>
+      </c>
+      <c r="N9" t="n">
+        <v>63</v>
+      </c>
+      <c r="O9" t="n">
+        <v>63</v>
+      </c>
+      <c r="P9" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>63</v>
+      </c>
+      <c r="R9" t="n">
+        <v>63</v>
+      </c>
+      <c r="S9" t="n">
+        <v>45</v>
+      </c>
+      <c r="T9" t="n">
+        <v>45</v>
+      </c>
+      <c r="U9" t="n">
+        <v>45</v>
+      </c>
+      <c r="V9" t="n">
+        <v>63</v>
+      </c>
+      <c r="W9" t="n">
+        <v>63</v>
+      </c>
+      <c r="X9" t="n">
+        <v>63</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>63</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>45</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>45</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>45</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>63</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Dodano zwiększanie rozmiaru kolumn
</commit_message>
<xml_diff>
--- a/pyxltext.xlsx
+++ b/pyxltext.xlsx
@@ -420,6 +420,55 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
+    <col width="30" customWidth="1" min="17" max="17"/>
+    <col width="30" customWidth="1" min="18" max="18"/>
+    <col width="30" customWidth="1" min="19" max="19"/>
+    <col width="30" customWidth="1" min="20" max="20"/>
+    <col width="30" customWidth="1" min="21" max="21"/>
+    <col width="30" customWidth="1" min="22" max="22"/>
+    <col width="30" customWidth="1" min="23" max="23"/>
+    <col width="30" customWidth="1" min="24" max="24"/>
+    <col width="30" customWidth="1" min="25" max="25"/>
+    <col width="30" customWidth="1" min="26" max="26"/>
+    <col width="30" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="30" customWidth="1" min="29" max="29"/>
+    <col width="30" customWidth="1" min="30" max="30"/>
+    <col width="30" customWidth="1" min="31" max="31"/>
+    <col width="30" customWidth="1" min="32" max="32"/>
+    <col width="30" customWidth="1" min="33" max="33"/>
+    <col width="30" customWidth="1" min="34" max="34"/>
+    <col width="30" customWidth="1" min="35" max="35"/>
+    <col width="30" customWidth="1" min="36" max="36"/>
+    <col width="30" customWidth="1" min="37" max="37"/>
+    <col width="30" customWidth="1" min="38" max="38"/>
+    <col width="30" customWidth="1" min="39" max="39"/>
+    <col width="30" customWidth="1" min="40" max="40"/>
+    <col width="30" customWidth="1" min="41" max="41"/>
+    <col width="30" customWidth="1" min="42" max="42"/>
+    <col width="30" customWidth="1" min="43" max="43"/>
+    <col width="30" customWidth="1" min="44" max="44"/>
+    <col width="30" customWidth="1" min="45" max="45"/>
+    <col width="30" customWidth="1" min="46" max="46"/>
+    <col width="30" customWidth="1" min="47" max="47"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">

</xml_diff>